<commit_message>
revision update part 1
</commit_message>
<xml_diff>
--- a/notebooks/GDP_calculations_US-NY_v3.xlsx
+++ b/notebooks/GDP_calculations_US-NY_v3.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakshamsoni/Library/Mobile Documents/com~apple~CloudDocs/Workspace/Research/THEMIS/code/THEMIS/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCF8BAA-C041-7D4B-AAB1-C7EF370E8001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B176A0E2-FEAE-5147-9E0C-259B6FA516CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20260" xr2:uid="{E833F4D3-7AF9-C94A-AE81-BD2CF03E641C}"/>
+    <workbookView xWindow="-26660" yWindow="720" windowWidth="33160" windowHeight="20220" xr2:uid="{E833F4D3-7AF9-C94A-AE81-BD2CF03E641C}"/>
   </bookViews>
   <sheets>
     <sheet name="Calculations NY" sheetId="2" r:id="rId1"/>
     <sheet name="Raw Data US" sheetId="4" r:id="rId2"/>
     <sheet name="Raw Data NY" sheetId="6" r:id="rId3"/>
     <sheet name="Data US GDP Growth" sheetId="9" r:id="rId4"/>
+    <sheet name="Data NY GDP Growth" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="201">
   <si>
     <t>year</t>
   </si>
@@ -128,9 +129,6 @@
     <t>US GDP Breakdown per quarter (Billions of Dollars)</t>
   </si>
   <si>
-    <t>Change in US GDP (Billions of Dollars)</t>
-  </si>
-  <si>
     <t>x</t>
   </si>
   <si>
@@ -609,13 +607,52 @@
   </si>
   <si>
     <t>average</t>
+  </si>
+  <si>
+    <t>SASUMMARY State annual summary statistics: personal income, GDP, consumer spending, price indexes, and employment</t>
+  </si>
+  <si>
+    <t>Real gross domestic product (GDP) (Millions of chained 2012 dollars) 1/</t>
+  </si>
+  <si>
+    <t>1/ Chained (2012) dollar series are calculated as the product of the chain-type quantity index and the 2012 current-dollar value of the corresponding series, divided by 100. Because the formula for the chain-type quantity indexes uses weights of more than one period, the corresponding chained-dollar estimates are usually not additive. The difference between the United States and sum-of-states reflects federal military and civilian activity located overseas, as well as the differences in source data used to estimate GDP by industry and the expenditures measure of real GDP.</t>
+  </si>
+  <si>
+    <t>Last updated: March 31, 2023.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">average = </t>
+  </si>
+  <si>
+    <t>year on year increase</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>natural rate of increase in GDP</t>
+  </si>
+  <si>
+    <t>Projected GDP (Billions of Dollars)</t>
+  </si>
+  <si>
+    <t>US GDP Impact (Billions of Dollars)</t>
+  </si>
+  <si>
+    <t>Projected GDP (Millions of Dollars)</t>
+  </si>
+  <si>
+    <t>US-NY</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -678,8 +715,38 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -697,8 +764,42 @@
         <bgColor indexed="12"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -721,11 +822,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -745,42 +932,52 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="2" xfId="1"/>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="2" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="60% - Accent3" xfId="3" builtinId="40"/>
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <b val="0"/>
@@ -872,10 +1069,10 @@
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{72703BBC-3F5E-0F48-807D-32C70C9D02CB}" name="year"/>
     <tableColumn id="2" xr3:uid="{3FFCE1A5-28A8-9A48-9716-70973425C397}" name="quarter"/>
-    <tableColumn id="3" xr3:uid="{114C25BD-A16C-0641-B0F6-C5768026715C}" name="C" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{50123A76-25EA-C54F-8361-4F713D91C0DB}" name="I" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{6966534B-56FB-DD4E-A859-37AB722BCB12}" name="G" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{45DDBAA8-4B70-3A46-BF85-CE0EAC71A409}" name="X" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{114C25BD-A16C-0641-B0F6-C5768026715C}" name="C" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{50123A76-25EA-C54F-8361-4F713D91C0DB}" name="I" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{6966534B-56FB-DD4E-A859-37AB722BCB12}" name="G" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{45DDBAA8-4B70-3A46-BF85-CE0EAC71A409}" name="X" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -898,52 +1095,6 @@
     <tableColumn id="5" xr3:uid="{361FF9D0-A246-404D-8C89-71FFF69B484A}" name="x">
       <calculatedColumnFormula>F8-F4</calculatedColumnFormula>
     </tableColumn>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{4B2914F5-D181-2B4F-B94C-A73987D422E3}" name="Table6" displayName="Table6" ref="A26:Q34" totalsRowShown="0">
-  <autoFilter ref="A26:Q34" xr:uid="{4B2914F5-D181-2B4F-B94C-A73987D422E3}"/>
-  <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{38CCF5F6-BA7E-BB4B-B4EB-013292275259}" name="year"/>
-    <tableColumn id="2" xr3:uid="{56355894-30CB-E445-9857-AC2DAD175A17}" name="quarter"/>
-    <tableColumn id="3" xr3:uid="{5D78FB4E-5B4F-9A49-BD96-DCF005D0BEB6}" name="US GDP (Billions of Dollars)" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{6334102B-E99B-6C4C-AA30-1EA7F315CE92}" name="Change in US GDP (Billions of Dollars)">
-      <calculatedColumnFormula>C27-C23</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="5" xr3:uid="{35EDB2E9-8A23-104E-87BB-D3DAE93645BF}" name="% change in US GDP">
-      <calculatedColumnFormula>D27/C23</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="6" xr3:uid="{09A74D85-87AC-2C4C-B4AD-D3F4DEE650BB}" name="NY GDP (Millions of Dollars)"/>
-    <tableColumn id="7" xr3:uid="{FA6136C9-547E-7743-80B0-1C3C94A79CDA}" name="change in NY GDP (Millions of Dollars)">
-      <calculatedColumnFormula>F27-F23</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="8" xr3:uid="{B7766EFE-E03F-9A4B-A3E7-D7C117D8437F}" name="% change in NY GDP">
-      <calculatedColumnFormula>G27/F23</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="9" xr3:uid="{217DF78A-0C5A-9044-ACA4-4FF8A1CE11B8}" name="% share of national GDP"/>
-    <tableColumn id="10" xr3:uid="{E70D5A45-4A94-024D-B11C-1CF70127402D}" name="c">
-      <calculatedColumnFormula>$I23*C11*($H27/$E27)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="11" xr3:uid="{D5E2768D-B448-4C47-89B1-BC9725DBC24E}" name="i">
-      <calculatedColumnFormula>$I23*D11*($H27/$E27)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="12" xr3:uid="{8AC96F0E-6709-6B4B-9491-A0C37B0AD30A}" name="g">
-      <calculatedColumnFormula>$I23*E11*($H27/$E27)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="13" xr3:uid="{205CAD23-BB6B-6A4F-9C2A-FA10549CDE18}" name="x"/>
-    <tableColumn id="14" xr3:uid="{DF8958FA-B552-A74A-99C5-7C2E1546269D}" name="c (readjusted monthly)">
-      <calculatedColumnFormula>ROUND(J27/(3*4), 1)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="15" xr3:uid="{E73653B2-CDB6-A848-ACD8-E5FAACEB136F}" name="i (readjusted monthly)">
-      <calculatedColumnFormula>ROUND(K27/(3*4), 1)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="16" xr3:uid="{F6BE65CB-F692-9D40-8703-587CBE594BA6}" name="g (readjusted monthly)">
-      <calculatedColumnFormula>ROUND(L27/(3*4), 1)</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="17" xr3:uid="{2A87B621-6D07-414C-AF2F-5A87DB2C7189}" name="x (readjusted monthly)"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1246,10 +1397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{021142B1-FD13-EA4C-AC21-7BA0E7411603}">
-  <dimension ref="A2:Q34"/>
+  <dimension ref="A2:S36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1260,7 +1411,7 @@
     <col min="5" max="5" width="20.33203125" customWidth="1"/>
     <col min="6" max="6" width="26.33203125" customWidth="1"/>
     <col min="7" max="7" width="34.6640625" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" customWidth="1"/>
+    <col min="8" max="8" width="30" customWidth="1"/>
     <col min="9" max="9" width="23.5" customWidth="1"/>
     <col min="10" max="10" width="18.33203125" customWidth="1"/>
     <col min="11" max="11" width="18.1640625" customWidth="1"/>
@@ -1282,7 +1433,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" s="1"/>
     </row>
@@ -1294,19 +1445,19 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
-        <v>35</v>
-      </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1316,20 +1467,20 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="9">
         <v>12955.7</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="9">
         <v>3484.3</v>
       </c>
-      <c r="E4" s="15">
+      <c r="E4" s="9">
         <v>3271</v>
       </c>
-      <c r="F4" s="15">
+      <c r="F4" s="9">
         <v>-903.6</v>
       </c>
       <c r="H4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1339,20 +1490,20 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="9">
         <v>13038.9</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="9">
         <v>3504.9</v>
       </c>
-      <c r="E5" s="15">
+      <c r="E5" s="9">
         <v>3313.8</v>
       </c>
-      <c r="F5" s="15">
+      <c r="F5" s="9">
         <v>-924.5</v>
       </c>
       <c r="H5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1362,20 +1513,20 @@
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="9">
         <v>13148.9</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="9">
         <v>3527.2</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="9">
         <v>3341.2</v>
       </c>
-      <c r="F6" s="15">
+      <c r="F6" s="9">
         <v>-909.4</v>
       </c>
       <c r="H6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1385,20 +1536,20 @@
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="9">
         <v>13225.6</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="9">
         <v>3454.4</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="9">
         <v>3360.9</v>
       </c>
-      <c r="F7" s="15">
+      <c r="F7" s="9">
         <v>-832.8</v>
       </c>
       <c r="H7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1408,20 +1559,20 @@
       <c r="B8">
         <v>1</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="9">
         <v>13016.8</v>
       </c>
-      <c r="D8" s="15">
+      <c r="D8" s="9">
         <v>3409.9</v>
       </c>
-      <c r="E8" s="15">
+      <c r="E8" s="9">
         <v>3387.9</v>
       </c>
-      <c r="F8" s="15">
+      <c r="F8" s="9">
         <v>-828.2</v>
       </c>
       <c r="H8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1431,20 +1582,20 @@
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="9">
         <v>11817.1</v>
       </c>
-      <c r="D9" s="15">
+      <c r="D9" s="9">
         <v>2884.2</v>
       </c>
-      <c r="E9" s="15">
+      <c r="E9" s="9">
         <v>3448</v>
       </c>
-      <c r="F9" s="15">
+      <c r="F9" s="9">
         <v>-767.3</v>
       </c>
       <c r="H9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1454,20 +1605,20 @@
       <c r="B10">
         <v>3</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="9">
         <v>12922.4</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="9">
         <v>3394.1</v>
       </c>
-      <c r="E10" s="15">
+      <c r="E10" s="9">
         <v>3395.9</v>
       </c>
-      <c r="F10" s="15">
+      <c r="F10" s="9">
         <v>-991.1</v>
       </c>
       <c r="H10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1477,34 +1628,34 @@
       <c r="B11">
         <v>4</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="9">
         <v>13046.6</v>
       </c>
-      <c r="D11" s="15">
+      <c r="D11" s="9">
         <v>3537.6</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="9">
         <v>3394.8</v>
       </c>
-      <c r="F11" s="15">
+      <c r="F11" s="9">
         <v>-1104</v>
       </c>
       <c r="H11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C12" s="8"/>
       <c r="H12" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1521,7 +1672,7 @@
         <v>3</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
@@ -1566,7 +1717,7 @@
         <v>157.20000000000005</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B17">
         <v>3</v>
       </c>
@@ -1587,7 +1738,7 @@
         <v>-81.700000000000045</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B18">
         <v>4</v>
       </c>
@@ -1608,437 +1759,558 @@
         <v>-271.20000000000005</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:17" s="5" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4" t="s">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A24" s="2"/>
+      <c r="D24" s="25"/>
+      <c r="E24" s="25" t="s">
+        <v>195</v>
+      </c>
+      <c r="F24" s="25" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A25" s="2"/>
+      <c r="D25" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="E25" s="26">
+        <v>2.2017798069047793E-2</v>
+      </c>
+      <c r="F25" s="26">
+        <v>1.8133969999999999E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" s="5" customFormat="1" ht="83" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="H25" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="I25" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="J25" s="4" t="s">
+      <c r="K27" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="L27" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="M27" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="K25" s="4" t="s">
+      <c r="N27" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="L25" s="4" t="s">
+      <c r="O27" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="M25" s="4" t="s">
+      <c r="P27" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="N25" s="4" t="s">
+      <c r="Q27" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="O25" s="4" t="s">
+      <c r="R27" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="P25" s="4" t="s">
+      <c r="S27" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="Q25" s="4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B28" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D28" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="F28" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>156</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>199</v>
+      </c>
+      <c r="I28" s="14" t="s">
+        <v>157</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="K28" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="L28" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="M28" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="N28" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="O28" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="E26" t="s">
-        <v>22</v>
-      </c>
-      <c r="F26" t="s">
-        <v>157</v>
-      </c>
-      <c r="G26" t="s">
-        <v>158</v>
-      </c>
-      <c r="H26" t="s">
-        <v>159</v>
-      </c>
-      <c r="I26" t="s">
-        <v>23</v>
-      </c>
-      <c r="J26" t="s">
+      <c r="P28" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q28" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="R28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="S28" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A29" s="16">
+        <v>2019</v>
+      </c>
+      <c r="B29" s="17">
         <v>1</v>
       </c>
-      <c r="K26" t="s">
+      <c r="C29" s="18">
+        <v>18835.400000000001</v>
+      </c>
+      <c r="D29" s="18"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="17">
+        <v>1485313.9</v>
+      </c>
+      <c r="H29" s="17"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="17"/>
+      <c r="K29" s="17">
+        <f>G29/(C29*1000)</f>
+        <v>7.8857571381547503E-2</v>
+      </c>
+      <c r="L29" s="17"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="17"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="17"/>
+      <c r="R29" s="17"/>
+      <c r="S29" s="19"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A30" s="20">
+        <v>2019</v>
+      </c>
+      <c r="B30" s="21">
         <v>2</v>
       </c>
-      <c r="L26" t="s">
+      <c r="C30" s="22">
+        <v>18962.2</v>
+      </c>
+      <c r="D30" s="22"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21">
+        <v>1504078.5</v>
+      </c>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21">
+        <f>G30/(C30*1000)</f>
+        <v>7.9319831032264185E-2</v>
+      </c>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="23"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A31" s="16">
+        <v>2019</v>
+      </c>
+      <c r="B31" s="17">
         <v>3</v>
       </c>
-      <c r="M26" t="s">
-        <v>30</v>
-      </c>
-      <c r="N26" t="s">
-        <v>24</v>
-      </c>
-      <c r="O26" t="s">
-        <v>25</v>
-      </c>
-      <c r="P26" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="C31" s="18">
+        <v>19130.900000000001</v>
+      </c>
+      <c r="D31" s="18"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17">
+        <v>1506282.5</v>
+      </c>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+      <c r="K31" s="17">
+        <f>G31/(C31*1000)</f>
+        <v>7.8735579612041251E-2</v>
+      </c>
+      <c r="L31" s="17"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="17"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="17"/>
+      <c r="Q31" s="17"/>
+      <c r="R31" s="17"/>
+      <c r="S31" s="19"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A32" s="20">
         <v>2019</v>
       </c>
-      <c r="B27">
+      <c r="B32" s="21">
+        <v>4</v>
+      </c>
+      <c r="C32" s="22">
+        <v>19215.7</v>
+      </c>
+      <c r="D32" s="22"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21">
+        <v>1507658.7</v>
+      </c>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21">
+        <f>G32/(C32*1000)</f>
+        <v>7.8459733447129171E-2</v>
+      </c>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="23"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A33" s="16">
+        <v>2020</v>
+      </c>
+      <c r="B33" s="17">
         <v>1</v>
       </c>
-      <c r="C27" s="15">
-        <v>18835.400000000001</v>
-      </c>
-      <c r="F27">
-        <v>1485313.9</v>
-      </c>
-      <c r="I27">
-        <f>F27/(C27*1000)</f>
-        <v>7.8857571381547503E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>2019</v>
-      </c>
-      <c r="B28">
+      <c r="C33" s="18">
+        <v>18989.900000000001</v>
+      </c>
+      <c r="D33" s="18">
+        <f>C29*(1+$E$25)</f>
+        <v>19250.114033749742</v>
+      </c>
+      <c r="E33" s="17">
+        <f>C33-D33</f>
+        <v>-260.21403374974034</v>
+      </c>
+      <c r="F33" s="17">
+        <f>E33/D33</f>
+        <v>-1.3517532067266049E-2</v>
+      </c>
+      <c r="G33" s="17">
+        <v>1489185.1</v>
+      </c>
+      <c r="H33" s="17">
+        <f>G29*(1+$F$25)</f>
+        <v>1512248.537703183</v>
+      </c>
+      <c r="I33" s="17">
+        <f>G33-H33</f>
+        <v>-23063.437703182921</v>
+      </c>
+      <c r="J33" s="17">
+        <f>I33/H33</f>
+        <v>-1.5251089439446166E-2</v>
+      </c>
+      <c r="K33" s="17"/>
+      <c r="L33" s="17">
+        <f t="shared" ref="L33:O36" si="1">$K29*C15*($J33/$F33)</f>
+        <v>5.4361078888447585</v>
+      </c>
+      <c r="M33" s="17">
+        <f t="shared" si="1"/>
+        <v>-6.6194177893626875</v>
+      </c>
+      <c r="N33" s="17">
+        <f t="shared" si="1"/>
+        <v>10.400671230866907</v>
+      </c>
+      <c r="O33" s="17">
+        <f t="shared" si="1"/>
+        <v>6.7083884585745412</v>
+      </c>
+      <c r="P33" s="17">
+        <f>ROUND(L33/(3*4), 1)</f>
+        <v>0.5</v>
+      </c>
+      <c r="Q33" s="17">
+        <f t="shared" ref="Q33:S36" si="2">ROUND(M33/(3*4), 1)</f>
+        <v>-0.6</v>
+      </c>
+      <c r="R33" s="17">
+        <f t="shared" si="2"/>
+        <v>0.9</v>
+      </c>
+      <c r="S33" s="19">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A34" s="20">
+        <v>2020</v>
+      </c>
+      <c r="B34" s="21">
         <v>2</v>
       </c>
-      <c r="C28" s="15">
-        <v>18962.2</v>
-      </c>
-      <c r="F28">
-        <v>1504078.5</v>
-      </c>
-      <c r="I28">
-        <f t="shared" ref="I28:I30" si="1">F28/(C28*1000)</f>
-        <v>7.9319831032264185E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>2019</v>
-      </c>
-      <c r="B29">
+      <c r="C34" s="22">
+        <v>17378.7</v>
+      </c>
+      <c r="D34" s="18">
+        <f t="shared" ref="D34:D36" si="3">C30*(1+$E$25)</f>
+        <v>19379.705890544898</v>
+      </c>
+      <c r="E34" s="17">
+        <f t="shared" ref="E34:E36" si="4">C34-D34</f>
+        <v>-2001.0058905448968</v>
+      </c>
+      <c r="F34" s="17">
+        <f t="shared" ref="F34:F36" si="5">E34/D34</f>
+        <v>-0.10325264489804054</v>
+      </c>
+      <c r="G34" s="21">
+        <v>1347704.9</v>
+      </c>
+      <c r="H34" s="17">
+        <f t="shared" ref="H34:H36" si="6">G30*(1+$F$25)</f>
+        <v>1531353.414396645</v>
+      </c>
+      <c r="I34" s="17">
+        <f t="shared" ref="I34:I36" si="7">G34-H34</f>
+        <v>-183648.51439664513</v>
+      </c>
+      <c r="J34" s="17">
+        <f t="shared" ref="J34:J36" si="8">I34/H34</f>
+        <v>-0.11992562439873022</v>
+      </c>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21">
+        <f t="shared" si="1"/>
+        <v>-112.56223409794215</v>
+      </c>
+      <c r="M34" s="21">
+        <f t="shared" si="1"/>
+        <v>-57.183973403660794</v>
+      </c>
+      <c r="N34" s="21">
+        <f t="shared" si="1"/>
+        <v>12.363604367280917</v>
+      </c>
+      <c r="O34" s="21">
+        <f t="shared" si="1"/>
+        <v>14.482552954817907</v>
+      </c>
+      <c r="P34" s="21">
+        <f t="shared" ref="P34:P36" si="9">ROUND(L34/(3*4), 1)</f>
+        <v>-9.4</v>
+      </c>
+      <c r="Q34" s="21">
+        <f t="shared" si="2"/>
+        <v>-4.8</v>
+      </c>
+      <c r="R34" s="21">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="S34" s="23">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A35" s="16">
+        <v>2020</v>
+      </c>
+      <c r="B35" s="17">
         <v>3</v>
       </c>
-      <c r="C29" s="15">
-        <v>19130.900000000001</v>
-      </c>
-      <c r="F29">
-        <v>1506282.5</v>
-      </c>
-      <c r="I29">
+      <c r="C35" s="18">
+        <v>18743.7</v>
+      </c>
+      <c r="D35" s="18">
+        <f t="shared" si="3"/>
+        <v>19552.120293079144</v>
+      </c>
+      <c r="E35" s="17">
+        <f t="shared" si="4"/>
+        <v>-808.42029307914345</v>
+      </c>
+      <c r="F35" s="17">
+        <f t="shared" si="5"/>
+        <v>-4.1346937363376371E-2</v>
+      </c>
+      <c r="G35" s="17">
+        <v>1442509.1</v>
+      </c>
+      <c r="H35" s="17">
+        <f t="shared" si="6"/>
+        <v>1533597.381666525</v>
+      </c>
+      <c r="I35" s="17">
+        <f t="shared" si="7"/>
+        <v>-91088.281666524941</v>
+      </c>
+      <c r="J35" s="17">
+        <f t="shared" si="8"/>
+        <v>-5.9395172915293712E-2</v>
+      </c>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17">
         <f t="shared" si="1"/>
-        <v>7.8735579612041251E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30">
-        <v>2019</v>
-      </c>
-      <c r="B30">
+        <v>-25.618107285894943</v>
+      </c>
+      <c r="M35" s="17">
+        <f t="shared" si="1"/>
+        <v>-15.054172537539138</v>
+      </c>
+      <c r="N35" s="17">
+        <f t="shared" si="1"/>
+        <v>6.1868011856002667</v>
+      </c>
+      <c r="O35" s="17">
+        <f t="shared" si="1"/>
+        <v>-9.2406152991506314</v>
+      </c>
+      <c r="P35" s="17">
+        <f t="shared" si="9"/>
+        <v>-2.1</v>
+      </c>
+      <c r="Q35" s="17">
+        <f t="shared" si="2"/>
+        <v>-1.3</v>
+      </c>
+      <c r="R35" s="17">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="S35" s="19">
+        <f t="shared" si="2"/>
+        <v>-0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A36" s="10">
+        <v>2020</v>
+      </c>
+      <c r="B36" s="11">
         <v>4</v>
       </c>
-      <c r="C30" s="15">
-        <v>19215.7</v>
-      </c>
-      <c r="F30">
-        <v>1507658.7</v>
-      </c>
-      <c r="I30">
+      <c r="C36" s="24">
+        <v>18924.3</v>
+      </c>
+      <c r="D36" s="18">
+        <f t="shared" si="3"/>
+        <v>19638.7874023554</v>
+      </c>
+      <c r="E36" s="17">
+        <f t="shared" si="4"/>
+        <v>-714.48740235540026</v>
+      </c>
+      <c r="F36" s="17">
+        <f t="shared" si="5"/>
+        <v>-3.6381441874038897E-2</v>
+      </c>
+      <c r="G36" s="11">
+        <v>1450628.9</v>
+      </c>
+      <c r="H36" s="17">
+        <f t="shared" si="6"/>
+        <v>1534998.5376360391</v>
+      </c>
+      <c r="I36" s="17">
+        <f t="shared" si="7"/>
+        <v>-84369.637636039173</v>
+      </c>
+      <c r="J36" s="17">
+        <f t="shared" si="8"/>
+        <v>-5.4963985676476208E-2</v>
+      </c>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11">
         <f t="shared" si="1"/>
-        <v>7.8459733447129171E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31">
-        <v>2020</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" s="15">
-        <v>18989.900000000001</v>
-      </c>
-      <c r="D31">
-        <f>C31-C27</f>
-        <v>154.5</v>
-      </c>
-      <c r="E31">
-        <f>D31/C27</f>
-        <v>8.2026397103326706E-3</v>
-      </c>
-      <c r="F31">
-        <v>1489185.1</v>
-      </c>
-      <c r="G31">
-        <f>F31-F27</f>
-        <v>3871.2000000001863</v>
-      </c>
-      <c r="H31">
-        <f>G31/F27</f>
-        <v>2.606317762191673E-3</v>
-      </c>
-      <c r="J31">
-        <f>$I27*C15*($H31/$E31)</f>
-        <v>1.530940582524309</v>
-      </c>
-      <c r="K31">
-        <f t="shared" ref="K31:M34" si="2">$I27*D15*($H31/$E31)</f>
-        <v>-1.8641895145631988</v>
-      </c>
-      <c r="L31">
+        <v>-21.217693426596522</v>
+      </c>
+      <c r="M36" s="11">
+        <f t="shared" si="1"/>
+        <v>9.8620787323621624</v>
+      </c>
+      <c r="N36" s="11">
+        <f t="shared" si="1"/>
+        <v>4.0183229450370055</v>
+      </c>
+      <c r="O36" s="11">
+        <f t="shared" si="1"/>
+        <v>-32.146583560295966</v>
+      </c>
+      <c r="P36" s="11">
+        <f t="shared" si="9"/>
+        <v>-1.8</v>
+      </c>
+      <c r="Q36" s="11">
         <f t="shared" si="2"/>
-        <v>2.9290827184467454</v>
-      </c>
-      <c r="M31">
+        <v>0.8</v>
+      </c>
+      <c r="R36" s="11">
         <f t="shared" si="2"/>
-        <v>1.8892458252428088</v>
-      </c>
-      <c r="N31">
-        <f>ROUND(J31/(3*4), 1)</f>
-        <v>0.1</v>
-      </c>
-      <c r="O31">
-        <f t="shared" ref="O31:Q34" si="3">ROUND(K31/(3*4), 1)</f>
-        <v>-0.2</v>
-      </c>
-      <c r="P31">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-      <c r="Q31">
-        <f t="shared" si="3"/>
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32">
-        <v>2020</v>
-      </c>
-      <c r="B32">
-        <v>2</v>
-      </c>
-      <c r="C32" s="15">
-        <v>17378.7</v>
-      </c>
-      <c r="D32">
-        <f t="shared" ref="D32:D34" si="4">C32-C28</f>
-        <v>-1583.5</v>
-      </c>
-      <c r="E32">
-        <f t="shared" ref="E32:E34" si="5">D32/C28</f>
-        <v>-8.3508242714452965E-2</v>
-      </c>
-      <c r="F32">
-        <v>1347704.9</v>
-      </c>
-      <c r="G32">
-        <f t="shared" ref="G32:G34" si="6">F32-F28</f>
-        <v>-156373.60000000009</v>
-      </c>
-      <c r="H32">
-        <f t="shared" ref="H32:H34" si="7">G32/F28</f>
-        <v>-0.10396638207380804</v>
-      </c>
-      <c r="J32">
-        <f t="shared" ref="J32:J34" si="8">$I28*C16*($H32/$E32)</f>
-        <v>-120.65504545626776</v>
-      </c>
-      <c r="K32">
+        <v>0.3</v>
+      </c>
+      <c r="S36" s="12">
         <f t="shared" si="2"/>
-        <v>-61.295291139880071</v>
-      </c>
-      <c r="L32">
-        <f t="shared" si="2"/>
-        <v>13.252502128197023</v>
-      </c>
-      <c r="M32">
-        <f t="shared" si="2"/>
-        <v>15.523795339437966</v>
-      </c>
-      <c r="N32">
-        <f t="shared" ref="N32:N34" si="9">ROUND(J32/(3*4), 1)</f>
-        <v>-10.1</v>
-      </c>
-      <c r="O32">
-        <f t="shared" si="3"/>
-        <v>-5.0999999999999996</v>
-      </c>
-      <c r="P32">
-        <f t="shared" si="3"/>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q32">
-        <f t="shared" si="3"/>
-        <v>1.3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33">
-        <v>2020</v>
-      </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33" s="15">
-        <v>18743.7</v>
-      </c>
-      <c r="D33">
-        <f t="shared" si="4"/>
-        <v>-387.20000000000073</v>
-      </c>
-      <c r="E33">
-        <f t="shared" si="5"/>
-        <v>-2.0239507811969155E-2</v>
-      </c>
-      <c r="F33">
-        <v>1442509.1</v>
-      </c>
-      <c r="G33">
-        <f t="shared" si="6"/>
-        <v>-63773.399999999907</v>
-      </c>
-      <c r="H33">
-        <f t="shared" si="7"/>
-        <v>-4.2338273199084439E-2</v>
-      </c>
-      <c r="J33">
-        <f t="shared" si="8"/>
-        <v>-37.305462551652766</v>
-      </c>
-      <c r="K33">
-        <f t="shared" si="2"/>
-        <v>-21.922106249999914</v>
-      </c>
-      <c r="L33">
-        <f t="shared" si="2"/>
-        <v>9.0093103822314209</v>
-      </c>
-      <c r="M33">
-        <f t="shared" si="2"/>
-        <v>-13.456319163223103</v>
-      </c>
-      <c r="N33">
-        <f t="shared" si="9"/>
-        <v>-3.1</v>
-      </c>
-      <c r="O33">
-        <f t="shared" si="3"/>
-        <v>-1.8</v>
-      </c>
-      <c r="P33">
-        <f t="shared" si="3"/>
-        <v>0.8</v>
-      </c>
-      <c r="Q33">
-        <f t="shared" si="3"/>
-        <v>-1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>2020</v>
-      </c>
-      <c r="B34">
-        <v>4</v>
-      </c>
-      <c r="C34" s="15">
-        <v>18924.3</v>
-      </c>
-      <c r="D34">
-        <f t="shared" si="4"/>
-        <v>-291.40000000000146</v>
-      </c>
-      <c r="E34">
-        <f t="shared" si="5"/>
-        <v>-1.5164683045634635E-2</v>
-      </c>
-      <c r="F34">
-        <v>1450628.9</v>
-      </c>
-      <c r="G34">
-        <f t="shared" si="6"/>
-        <v>-57029.800000000047</v>
-      </c>
-      <c r="H34">
-        <f t="shared" si="7"/>
-        <v>-3.7826730943813773E-2</v>
-      </c>
-      <c r="J34">
-        <f t="shared" si="8"/>
-        <v>-35.032032258064369</v>
-      </c>
-      <c r="K34">
-        <f t="shared" si="2"/>
-        <v>16.283045161290218</v>
-      </c>
-      <c r="L34">
-        <f t="shared" si="2"/>
-        <v>6.634558064516118</v>
-      </c>
-      <c r="M34">
-        <f t="shared" si="2"/>
-        <v>-53.076464516128816</v>
-      </c>
-      <c r="N34">
-        <f t="shared" si="9"/>
-        <v>-2.9</v>
-      </c>
-      <c r="O34">
-        <f t="shared" si="3"/>
-        <v>1.4</v>
-      </c>
-      <c r="P34">
-        <f t="shared" si="3"/>
-        <v>0.6</v>
-      </c>
-      <c r="Q34">
-        <f t="shared" si="3"/>
-        <v>-4.4000000000000004</v>
+        <v>-2.7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="3">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2054,84 +2326,84 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+    </row>
+    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
         <v>170</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-    </row>
-    <row r="2" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
+      <c r="A3" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
+      <c r="A4" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
-      <c r="G6" s="12" t="s">
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="H6" s="12"/>
-      <c r="I6" s="12"/>
-      <c r="J6" s="12"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="12"/>
+      <c r="A7" s="35"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="6" t="s">
         <v>8</v>
       </c>
@@ -2159,7 +2431,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>12</v>
@@ -2191,10 +2463,10 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="7">
         <v>12955.7</v>
@@ -2223,10 +2495,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10">
         <v>4623.6000000000004</v>
@@ -2255,10 +2527,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
         <v>113</v>
-      </c>
-      <c r="B11" t="s">
-        <v>114</v>
       </c>
       <c r="C11">
         <v>1683.2</v>
@@ -2287,10 +2559,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
         <v>115</v>
-      </c>
-      <c r="B12" t="s">
-        <v>116</v>
       </c>
       <c r="C12">
         <v>2951</v>
@@ -2319,10 +2591,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13">
         <v>8365.1</v>
@@ -2351,10 +2623,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="C14" s="7">
         <v>3484.3</v>
@@ -2383,10 +2655,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" t="s">
         <v>120</v>
-      </c>
-      <c r="B15" t="s">
-        <v>121</v>
       </c>
       <c r="C15">
         <v>3351.5</v>
@@ -2415,10 +2687,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" t="s">
         <v>122</v>
-      </c>
-      <c r="B16" t="s">
-        <v>123</v>
       </c>
       <c r="C16">
         <v>2762.1</v>
@@ -2447,10 +2719,10 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C17">
         <v>543.4</v>
@@ -2479,10 +2751,10 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C18">
         <v>1250.0999999999999</v>
@@ -2511,10 +2783,10 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C19">
         <v>975.7</v>
@@ -2543,10 +2815,10 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C20">
         <v>596</v>
@@ -2575,10 +2847,10 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" t="s">
         <v>128</v>
-      </c>
-      <c r="B21" t="s">
-        <v>129</v>
       </c>
       <c r="C21">
         <v>134.6</v>
@@ -2607,10 +2879,10 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="C22" s="7">
         <v>-903.6</v>
@@ -2639,10 +2911,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" t="s">
         <v>132</v>
-      </c>
-      <c r="B23" t="s">
-        <v>133</v>
       </c>
       <c r="C23">
         <v>2582.3000000000002</v>
@@ -2671,10 +2943,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" t="s">
         <v>134</v>
-      </c>
-      <c r="B24" t="s">
-        <v>135</v>
       </c>
       <c r="C24">
         <v>1813</v>
@@ -2703,10 +2975,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" t="s">
         <v>136</v>
-      </c>
-      <c r="B25" t="s">
-        <v>137</v>
       </c>
       <c r="C25">
         <v>774.5</v>
@@ -2735,10 +3007,10 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" t="s">
         <v>138</v>
-      </c>
-      <c r="B26" t="s">
-        <v>139</v>
       </c>
       <c r="C26">
         <v>3485.9</v>
@@ -2767,10 +3039,10 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C27">
         <v>2939.7</v>
@@ -2799,10 +3071,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C28">
         <v>549.79999999999995</v>
@@ -2831,10 +3103,10 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="C29" s="7">
         <v>3271</v>
@@ -2863,10 +3135,10 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" t="s">
         <v>144</v>
-      </c>
-      <c r="B30" t="s">
-        <v>145</v>
       </c>
       <c r="C30">
         <v>1255.5999999999999</v>
@@ -2895,10 +3167,10 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" t="s">
         <v>146</v>
-      </c>
-      <c r="B31" t="s">
-        <v>147</v>
       </c>
       <c r="C31">
         <v>771.3</v>
@@ -2927,10 +3199,10 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C32">
         <v>484.5</v>
@@ -2959,10 +3231,10 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C33">
         <v>2014</v>
@@ -2991,10 +3263,10 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" t="s">
         <v>172</v>
-      </c>
-      <c r="B34" t="s">
-        <v>173</v>
       </c>
       <c r="C34">
         <v>-31.6</v>
@@ -3022,38 +3294,37 @@
       </c>
     </row>
     <row r="35" spans="1:11" ht="17" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
+      <c r="A35" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
+      <c r="A36" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A35:K35"/>
     <mergeCell ref="A36:K36"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="B6:B7"/>
@@ -3063,6 +3334,7 @@
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A3:J3"/>
     <mergeCell ref="A4:J4"/>
+    <mergeCell ref="A35:K35"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3079,81 +3351,81 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:12" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="30" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+    </row>
+    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-    </row>
-    <row r="2" spans="1:12" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>13</v>
@@ -3182,16 +3454,16 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" t="s">
         <v>153</v>
       </c>
-      <c r="B7" t="s">
-        <v>154</v>
-      </c>
       <c r="C7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" t="s">
         <v>56</v>
-      </c>
-      <c r="D7" t="s">
-        <v>57</v>
       </c>
       <c r="E7">
         <v>1485313.9</v>
@@ -3220,16 +3492,16 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" t="s">
         <v>153</v>
       </c>
-      <c r="B8" t="s">
-        <v>154</v>
-      </c>
       <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" t="s">
         <v>58</v>
-      </c>
-      <c r="D8" t="s">
-        <v>59</v>
       </c>
       <c r="E8">
         <v>1332303.3999999999</v>
@@ -3258,16 +3530,16 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" t="s">
         <v>153</v>
       </c>
-      <c r="B9" t="s">
-        <v>154</v>
-      </c>
       <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
         <v>60</v>
-      </c>
-      <c r="D9" t="s">
-        <v>61</v>
       </c>
       <c r="E9">
         <v>4218.8</v>
@@ -3296,16 +3568,16 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" t="s">
         <v>153</v>
       </c>
-      <c r="B10" t="s">
-        <v>154</v>
-      </c>
       <c r="C10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D10" t="s">
         <v>62</v>
-      </c>
-      <c r="D10" t="s">
-        <v>63</v>
       </c>
       <c r="E10">
         <v>1084.0999999999999</v>
@@ -3334,16 +3606,16 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B11" t="s">
         <v>153</v>
       </c>
-      <c r="B11" t="s">
-        <v>154</v>
-      </c>
       <c r="C11" t="s">
+        <v>63</v>
+      </c>
+      <c r="D11" t="s">
         <v>64</v>
-      </c>
-      <c r="D11" t="s">
-        <v>65</v>
       </c>
       <c r="E11">
         <v>20969.400000000001</v>
@@ -3372,16 +3644,16 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>152</v>
+      </c>
+      <c r="B12" t="s">
         <v>153</v>
       </c>
-      <c r="B12" t="s">
-        <v>154</v>
-      </c>
       <c r="C12" t="s">
+        <v>65</v>
+      </c>
+      <c r="D12" t="s">
         <v>66</v>
-      </c>
-      <c r="D12" t="s">
-        <v>67</v>
       </c>
       <c r="E12">
         <v>42644.3</v>
@@ -3410,16 +3682,16 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>152</v>
+      </c>
+      <c r="B13" t="s">
         <v>153</v>
       </c>
-      <c r="B13" t="s">
-        <v>154</v>
-      </c>
       <c r="C13" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" t="s">
         <v>68</v>
-      </c>
-      <c r="D13" t="s">
-        <v>69</v>
       </c>
       <c r="E13">
         <v>66676.899999999994</v>
@@ -3448,16 +3720,16 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" t="s">
         <v>153</v>
       </c>
-      <c r="B14" t="s">
-        <v>154</v>
-      </c>
       <c r="C14" t="s">
+        <v>69</v>
+      </c>
+      <c r="D14" t="s">
         <v>70</v>
-      </c>
-      <c r="D14" t="s">
-        <v>71</v>
       </c>
       <c r="E14">
         <v>34015.800000000003</v>
@@ -3486,16 +3758,16 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>152</v>
+      </c>
+      <c r="B15" t="s">
         <v>153</v>
       </c>
-      <c r="B15" t="s">
-        <v>154</v>
-      </c>
       <c r="C15" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" t="s">
         <v>72</v>
-      </c>
-      <c r="D15" t="s">
-        <v>73</v>
       </c>
       <c r="E15">
         <v>32607.599999999999</v>
@@ -3524,16 +3796,16 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" t="s">
         <v>153</v>
       </c>
-      <c r="B16" t="s">
-        <v>154</v>
-      </c>
       <c r="C16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D16" t="s">
         <v>74</v>
-      </c>
-      <c r="D16" t="s">
-        <v>75</v>
       </c>
       <c r="E16">
         <v>67744.5</v>
@@ -3562,16 +3834,16 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
+        <v>152</v>
+      </c>
+      <c r="B17" t="s">
         <v>153</v>
       </c>
-      <c r="B17" t="s">
-        <v>154</v>
-      </c>
       <c r="C17" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" t="s">
         <v>76</v>
-      </c>
-      <c r="D17" t="s">
-        <v>77</v>
       </c>
       <c r="E17">
         <v>74483.5</v>
@@ -3600,16 +3872,16 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
+        <v>152</v>
+      </c>
+      <c r="B18" t="s">
         <v>153</v>
       </c>
-      <c r="B18" t="s">
-        <v>154</v>
-      </c>
       <c r="C18" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" t="s">
         <v>78</v>
-      </c>
-      <c r="D18" t="s">
-        <v>79</v>
       </c>
       <c r="E18">
         <v>31003.8</v>
@@ -3638,16 +3910,16 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B19" t="s">
         <v>153</v>
       </c>
-      <c r="B19" t="s">
-        <v>154</v>
-      </c>
       <c r="C19" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" t="s">
         <v>80</v>
-      </c>
-      <c r="D19" t="s">
-        <v>81</v>
       </c>
       <c r="E19">
         <v>160423.79999999999</v>
@@ -3676,16 +3948,16 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20" t="s">
         <v>153</v>
       </c>
-      <c r="B20" t="s">
-        <v>154</v>
-      </c>
       <c r="C20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" t="s">
         <v>82</v>
-      </c>
-      <c r="D20" t="s">
-        <v>83</v>
       </c>
       <c r="E20">
         <v>234094.2</v>
@@ -3714,16 +3986,16 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>152</v>
+      </c>
+      <c r="B21" t="s">
         <v>153</v>
       </c>
-      <c r="B21" t="s">
-        <v>154</v>
-      </c>
       <c r="C21" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" t="s">
         <v>84</v>
-      </c>
-      <c r="D21" t="s">
-        <v>85</v>
       </c>
       <c r="E21">
         <v>193724.79999999999</v>
@@ -3752,16 +4024,16 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>152</v>
+      </c>
+      <c r="B22" t="s">
         <v>153</v>
       </c>
-      <c r="B22" t="s">
-        <v>154</v>
-      </c>
       <c r="C22" t="s">
+        <v>85</v>
+      </c>
+      <c r="D22" t="s">
         <v>86</v>
-      </c>
-      <c r="D22" t="s">
-        <v>87</v>
       </c>
       <c r="E22">
         <v>134437.1</v>
@@ -3790,16 +4062,16 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>152</v>
+      </c>
+      <c r="B23" t="s">
         <v>153</v>
       </c>
-      <c r="B23" t="s">
-        <v>154</v>
-      </c>
       <c r="C23" t="s">
+        <v>87</v>
+      </c>
+      <c r="D23" t="s">
         <v>88</v>
-      </c>
-      <c r="D23" t="s">
-        <v>89</v>
       </c>
       <c r="E23">
         <v>30666.5</v>
@@ -3828,16 +4100,16 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>152</v>
+      </c>
+      <c r="B24" t="s">
         <v>153</v>
       </c>
-      <c r="B24" t="s">
-        <v>154</v>
-      </c>
       <c r="C24" t="s">
+        <v>89</v>
+      </c>
+      <c r="D24" t="s">
         <v>90</v>
-      </c>
-      <c r="D24" t="s">
-        <v>91</v>
       </c>
       <c r="E24">
         <v>43028.2</v>
@@ -3866,16 +4138,16 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>152</v>
+      </c>
+      <c r="B25" t="s">
         <v>153</v>
       </c>
-      <c r="B25" t="s">
-        <v>154</v>
-      </c>
       <c r="C25" t="s">
+        <v>91</v>
+      </c>
+      <c r="D25" t="s">
         <v>92</v>
-      </c>
-      <c r="D25" t="s">
-        <v>93</v>
       </c>
       <c r="E25">
         <v>30927.599999999999</v>
@@ -3904,16 +4176,16 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>152</v>
+      </c>
+      <c r="B26" t="s">
         <v>153</v>
       </c>
-      <c r="B26" t="s">
-        <v>154</v>
-      </c>
       <c r="C26" t="s">
+        <v>93</v>
+      </c>
+      <c r="D26" t="s">
         <v>94</v>
-      </c>
-      <c r="D26" t="s">
-        <v>95</v>
       </c>
       <c r="E26">
         <v>113822.5</v>
@@ -3942,16 +4214,16 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>152</v>
+      </c>
+      <c r="B27" t="s">
         <v>153</v>
       </c>
-      <c r="B27" t="s">
-        <v>154</v>
-      </c>
       <c r="C27" t="s">
+        <v>95</v>
+      </c>
+      <c r="D27" t="s">
         <v>96</v>
-      </c>
-      <c r="D27" t="s">
-        <v>97</v>
       </c>
       <c r="E27">
         <v>25004.400000000001</v>
@@ -3980,16 +4252,16 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>152</v>
+      </c>
+      <c r="B28" t="s">
         <v>153</v>
       </c>
-      <c r="B28" t="s">
-        <v>154</v>
-      </c>
       <c r="C28" t="s">
+        <v>97</v>
+      </c>
+      <c r="D28" t="s">
         <v>98</v>
-      </c>
-      <c r="D28" t="s">
-        <v>99</v>
       </c>
       <c r="E28">
         <v>42005.4</v>
@@ -4018,16 +4290,16 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B29" t="s">
         <v>153</v>
       </c>
-      <c r="B29" t="s">
-        <v>154</v>
-      </c>
       <c r="C29" t="s">
+        <v>99</v>
+      </c>
+      <c r="D29" t="s">
         <v>100</v>
-      </c>
-      <c r="D29" t="s">
-        <v>101</v>
       </c>
       <c r="E29">
         <v>27306.7</v>
@@ -4056,16 +4328,16 @@
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>152</v>
+      </c>
+      <c r="B30" t="s">
         <v>153</v>
       </c>
-      <c r="B30" t="s">
-        <v>154</v>
-      </c>
       <c r="C30" t="s">
+        <v>101</v>
+      </c>
+      <c r="D30" t="s">
         <v>102</v>
-      </c>
-      <c r="D30" t="s">
-        <v>103</v>
       </c>
       <c r="E30">
         <v>153183.6</v>
@@ -4094,16 +4366,16 @@
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>152</v>
+      </c>
+      <c r="B31" t="s">
         <v>153</v>
       </c>
-      <c r="B31" t="s">
-        <v>154</v>
-      </c>
       <c r="C31" t="s">
+        <v>103</v>
+      </c>
+      <c r="D31" t="s">
         <v>104</v>
-      </c>
-      <c r="D31" t="s">
-        <v>105</v>
       </c>
       <c r="E31">
         <v>17267.900000000001</v>
@@ -4132,16 +4404,16 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>152</v>
+      </c>
+      <c r="B32" t="s">
         <v>153</v>
       </c>
-      <c r="B32" t="s">
-        <v>154</v>
-      </c>
       <c r="C32" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" t="s">
         <v>106</v>
-      </c>
-      <c r="D32" t="s">
-        <v>107</v>
       </c>
       <c r="E32">
         <v>4560.8999999999996</v>
@@ -4170,16 +4442,16 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>152</v>
+      </c>
+      <c r="B33" t="s">
         <v>153</v>
       </c>
-      <c r="B33" t="s">
-        <v>154</v>
-      </c>
       <c r="C33" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" t="s">
         <v>108</v>
-      </c>
-      <c r="D33" t="s">
-        <v>109</v>
       </c>
       <c r="E33">
         <v>131236.6</v>
@@ -4207,55 +4479,55 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.25">
-      <c r="A34" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
-      <c r="F34" s="10"/>
-      <c r="G34" s="10"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10"/>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="10"/>
-      <c r="M34" s="10"/>
+      <c r="A34" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
+      <c r="M34" s="31"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A35" s="13" t="s">
-        <v>177</v>
-      </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
+      <c r="A35" s="34" t="s">
+        <v>176</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A36" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
+      <c r="A36" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -4273,126 +4545,126 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E01EC2-16B4-974D-AF63-642E08D85865}">
-  <dimension ref="A1:P39"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+      <selection activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:13" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
+      <c r="A1" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
     </row>
     <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
+      <c r="A2" s="32" t="s">
+        <v>177</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
+      <c r="A3" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>169</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
+      <c r="A4" s="31" t="s">
+        <v>168</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="E6" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="F6" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="G6" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="H6" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="I6" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="J6" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="K6" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="K6" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="L6" s="6" t="s">
+      <c r="L6" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="M6" s="27" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B7" t="s">
         <v>5</v>
@@ -4427,13 +4699,13 @@
       <c r="L7" t="s">
         <v>5</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="28" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" s="7" t="s">
         <v>12</v>
@@ -4465,19 +4737,19 @@
       <c r="K8" s="7">
         <v>18609.099999999999</v>
       </c>
-      <c r="L8" s="7">
+      <c r="L8">
         <v>19036.099999999999</v>
       </c>
-      <c r="M8" s="7">
+      <c r="M8" s="28">
         <v>18509.099999999999</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C9" s="7">
         <v>10716</v>
@@ -4506,19 +4778,19 @@
       <c r="K9" s="7">
         <v>12837.3</v>
       </c>
-      <c r="L9" s="7">
+      <c r="L9">
         <v>13092.3</v>
       </c>
-      <c r="M9" s="7">
+      <c r="M9" s="28">
         <v>12700.7</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C10">
         <v>3485.7</v>
@@ -4550,16 +4822,16 @@
       <c r="L10">
         <v>4711.6000000000004</v>
       </c>
-      <c r="M10">
+      <c r="M10" s="28">
         <v>4955.7</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
         <v>113</v>
-      </c>
-      <c r="B11" t="s">
-        <v>114</v>
       </c>
       <c r="C11">
         <v>1027.3</v>
@@ -4591,16 +4863,16 @@
       <c r="L11">
         <v>1740.1</v>
       </c>
-      <c r="M11">
+      <c r="M11" s="28">
         <v>1914.2</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
         <v>115</v>
-      </c>
-      <c r="B12" t="s">
-        <v>116</v>
       </c>
       <c r="C12">
         <v>2461.3000000000002</v>
@@ -4632,16 +4904,16 @@
       <c r="L12">
         <v>2985.4</v>
       </c>
-      <c r="M12">
+      <c r="M12" s="28">
         <v>3066.7</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13">
         <v>7230.4</v>
@@ -4673,16 +4945,16 @@
       <c r="L13">
         <v>8421</v>
       </c>
-      <c r="M13">
+      <c r="M13" s="28">
         <v>7863</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="C14" s="7">
         <v>2216.5</v>
@@ -4711,19 +4983,19 @@
       <c r="K14" s="7">
         <v>3398.9</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14">
         <v>3492.7</v>
       </c>
-      <c r="M14" s="7">
+      <c r="M14" s="28">
         <v>3306.5</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>119</v>
+      </c>
+      <c r="B15" t="s">
         <v>120</v>
-      </c>
-      <c r="B15" t="s">
-        <v>121</v>
       </c>
       <c r="C15">
         <v>2164.1999999999998</v>
@@ -4755,16 +5027,16 @@
       <c r="L15">
         <v>3404.2</v>
       </c>
-      <c r="M15">
+      <c r="M15" s="28">
         <v>3326.8</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>121</v>
+      </c>
+      <c r="B16" t="s">
         <v>122</v>
-      </c>
-      <c r="B16" t="s">
-        <v>123</v>
       </c>
       <c r="C16">
         <v>1781</v>
@@ -4796,16 +5068,16 @@
       <c r="L16">
         <v>2804.6</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="28">
         <v>2666</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C17">
         <v>412.8</v>
@@ -4837,16 +5109,16 @@
       <c r="L17">
         <v>567.9</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="28">
         <v>510.4</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C18">
         <v>781.2</v>
@@ -4878,16 +5150,16 @@
       <c r="L18">
         <v>1236.5</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="28">
         <v>1107.3</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C19">
         <v>588.1</v>
@@ -4919,16 +5191,16 @@
       <c r="L19">
         <v>1003.2</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="28">
         <v>1051.2</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C20">
         <v>383</v>
@@ -4960,16 +5232,16 @@
       <c r="L20">
         <v>606.20000000000005</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="28">
         <v>649.79999999999995</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B21" t="s">
         <v>128</v>
-      </c>
-      <c r="B21" t="s">
-        <v>129</v>
       </c>
       <c r="C21">
         <v>57.3</v>
@@ -5001,16 +5273,16 @@
       <c r="L21">
         <v>73.099999999999994</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="28">
         <v>-54.6</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>129</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>130</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>131</v>
       </c>
       <c r="C22" s="7">
         <v>-589.4</v>
@@ -5039,19 +5311,19 @@
       <c r="K22" s="7">
         <v>-865.4</v>
       </c>
-      <c r="L22" s="7">
+      <c r="L22">
         <v>-892.6</v>
       </c>
-      <c r="M22" s="7">
+      <c r="M22" s="28">
         <v>-922.6</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
+        <v>131</v>
+      </c>
+      <c r="B23" t="s">
         <v>132</v>
-      </c>
-      <c r="B23" t="s">
-        <v>133</v>
       </c>
       <c r="C23">
         <v>1989.5</v>
@@ -5083,16 +5355,16 @@
       <c r="L23">
         <v>2572.1</v>
       </c>
-      <c r="M23">
+      <c r="M23" s="28">
         <v>2231.6999999999998</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" t="s">
         <v>134</v>
-      </c>
-      <c r="B24" t="s">
-        <v>135</v>
       </c>
       <c r="C24">
         <v>1369.4</v>
@@ -5124,16 +5396,16 @@
       <c r="L24">
         <v>1791.5</v>
       </c>
-      <c r="M24">
+      <c r="M24" s="28">
         <v>1609.7</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
+        <v>135</v>
+      </c>
+      <c r="B25" t="s">
         <v>136</v>
-      </c>
-      <c r="B25" t="s">
-        <v>137</v>
       </c>
       <c r="C25">
         <v>620.1</v>
@@ -5165,16 +5437,16 @@
       <c r="L25">
         <v>783.1</v>
       </c>
-      <c r="M25">
+      <c r="M25" s="28">
         <v>635.79999999999995</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" t="s">
         <v>138</v>
-      </c>
-      <c r="B26" t="s">
-        <v>139</v>
       </c>
       <c r="C26">
         <v>2578.9</v>
@@ -5206,16 +5478,16 @@
       <c r="L26">
         <v>3464.7</v>
       </c>
-      <c r="M26">
+      <c r="M26" s="28">
         <v>3154.3</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C27">
         <v>2117.3000000000002</v>
@@ -5247,16 +5519,16 @@
       <c r="L27">
         <v>2913.5</v>
       </c>
-      <c r="M27">
+      <c r="M27" s="28">
         <v>2744.6</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B28" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C28">
         <v>461.5</v>
@@ -5288,16 +5560,16 @@
       <c r="L28">
         <v>552.9</v>
       </c>
-      <c r="M28">
+      <c r="M28" s="28">
         <v>431.3</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
+        <v>141</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>142</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>143</v>
       </c>
       <c r="C29" s="7">
         <v>3308</v>
@@ -5326,19 +5598,19 @@
       <c r="K29" s="7">
         <v>3215.3</v>
       </c>
-      <c r="L29" s="7">
+      <c r="L29">
         <v>3321.7</v>
       </c>
-      <c r="M29" s="7">
+      <c r="M29" s="28">
         <v>3406.7</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" t="s">
         <v>144</v>
-      </c>
-      <c r="B30" t="s">
-        <v>145</v>
       </c>
       <c r="C30">
         <v>1348.4</v>
@@ -5370,16 +5642,16 @@
       <c r="L30">
         <v>1279.3</v>
       </c>
-      <c r="M30">
+      <c r="M30" s="28">
         <v>1358.9</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" t="s">
         <v>146</v>
-      </c>
-      <c r="B31" t="s">
-        <v>147</v>
       </c>
       <c r="C31">
         <v>861.3</v>
@@ -5411,16 +5683,16 @@
       <c r="L31">
         <v>778.5</v>
       </c>
-      <c r="M31">
+      <c r="M31" s="28">
         <v>801.1</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C32">
         <v>487</v>
@@ -5452,16 +5724,16 @@
       <c r="L32">
         <v>500.7</v>
       </c>
-      <c r="M32">
+      <c r="M32" s="28">
         <v>556.6</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C33">
         <v>1959.8</v>
@@ -5493,16 +5765,16 @@
       <c r="L33">
         <v>2041.1</v>
       </c>
-      <c r="M33">
+      <c r="M33" s="28">
         <v>2048.5</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" t="s">
         <v>172</v>
-      </c>
-      <c r="B34" t="s">
-        <v>173</v>
       </c>
       <c r="C34">
         <v>-11.3</v>
@@ -5534,56 +5806,56 @@
       <c r="L34">
         <v>-26</v>
       </c>
-      <c r="M34">
+      <c r="M34" s="28">
         <v>-74.599999999999994</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="17" x14ac:dyDescent="0.25">
-      <c r="A35" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A36" s="13" t="s">
-        <v>174</v>
-      </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10"/>
-      <c r="I36" s="10"/>
-      <c r="J36" s="10"/>
-      <c r="K36" s="10"/>
-      <c r="L36" s="10"/>
-      <c r="M36" s="10"/>
-      <c r="N36" s="10"/>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.25">
+      <c r="A35" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="31"/>
+      <c r="N35" s="31"/>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A36" s="34" t="s">
+        <v>173</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="31"/>
+      <c r="N36" s="31"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D39">
         <f>(D8-C8)/C8</f>
         <v>1.5496197840117579E-2</v>
       </c>
       <c r="E39">
-        <f t="shared" ref="E39:M39" si="0">(E8-D8)/D8</f>
+        <f t="shared" ref="E39:L39" si="0">(E8-D8)/D8</f>
         <v>2.2810936664254475E-2</v>
       </c>
       <c r="F39">
@@ -5614,26 +5886,300 @@
         <f t="shared" si="0"/>
         <v>2.2945763094400055E-2</v>
       </c>
-      <c r="M39">
-        <f t="shared" si="0"/>
-        <v>-2.7684242045376943E-2</v>
-      </c>
-      <c r="O39" t="s">
-        <v>189</v>
-      </c>
-      <c r="P39">
-        <f>AVERAGE(D39:M39)</f>
-        <v>1.7047594057605319E-2</v>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="J40" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="K40" s="29">
+        <f>AVERAGE(D39:L39)</f>
+        <v>2.2017798069047793E-2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="A36:N36"/>
     <mergeCell ref="A1:M1"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:M3"/>
     <mergeCell ref="A4:M4"/>
     <mergeCell ref="A35:N35"/>
-    <mergeCell ref="A36:N36"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BC58EF8-B98F-4547-9E52-9BDCC0E1E9A4}">
+  <dimension ref="A1:P12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P12" sqref="P12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="30" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="31"/>
+      <c r="K1" s="31"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+    </row>
+    <row r="2" spans="1:16" ht="17" x14ac:dyDescent="0.2">
+      <c r="A2" s="32" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="31" t="s">
+        <v>150</v>
+      </c>
+      <c r="B4" s="31"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="31"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="L6" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>152</v>
+      </c>
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7">
+        <v>1277466.8</v>
+      </c>
+      <c r="D7">
+        <v>1279527.1000000001</v>
+      </c>
+      <c r="E7">
+        <v>1328233.5</v>
+      </c>
+      <c r="F7">
+        <v>1329376.3</v>
+      </c>
+      <c r="G7">
+        <v>1353410.4</v>
+      </c>
+      <c r="H7">
+        <v>1373643</v>
+      </c>
+      <c r="I7">
+        <v>1403230.5</v>
+      </c>
+      <c r="J7">
+        <v>1419112.1</v>
+      </c>
+      <c r="K7">
+        <v>1458382.4</v>
+      </c>
+      <c r="L7">
+        <v>1500833.4</v>
+      </c>
+      <c r="M7" s="28">
+        <v>1432507</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="17" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>151</v>
+      </c>
+      <c r="B8" s="31"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="31"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="31"/>
+      <c r="L8" s="31"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="31"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="34" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="31"/>
+      <c r="C9" s="31"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="31"/>
+      <c r="J9" s="31"/>
+      <c r="K9" s="31"/>
+      <c r="L9" s="31"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="31"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="34" t="s">
+        <v>192</v>
+      </c>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D12">
+        <f>(D7-C7)/C7</f>
+        <v>1.6128012093935017E-3</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ref="E12:L12" si="0">(E7-D7)/D7</f>
+        <v>3.8065938579964348E-2</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>8.6039088759622953E-4</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="0"/>
+        <v>1.8079230087071553E-2</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>1.4949345741690838E-2</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>2.1539439286626876E-2</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>1.1317883982709963E-2</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="0"/>
+        <v>2.7672443917573397E-2</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>2.9108277774059811E-2</v>
+      </c>
+      <c r="O12" t="s">
+        <v>193</v>
+      </c>
+      <c r="P12">
+        <f>AVERAGE(D12:L12)</f>
+        <v>1.8133972385187391E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A9:N9"/>
+    <mergeCell ref="A10:N10"/>
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A4:M4"/>
+    <mergeCell ref="A8:N8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>